<commit_message>
Ajuste subida de certificados masivos, correcion de nombres en labels, arreglo de bug en filtros de certificates y deliverys
</commit_message>
<xml_diff>
--- a/src/assets/MASIVO.xlsx
+++ b/src/assets/MASIVO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JUEGOS\PROJECTS\proyecto\WEB\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\memoj\OneDrive\Documents\YouTubeDownloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Estados" sheetId="3" r:id="rId2"/>
+    <sheet name="Tipos" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>NO_CERTIFICADO</t>
   </si>
@@ -48,13 +50,43 @@
   </si>
   <si>
     <t>FECHAESTADORUAF</t>
+  </si>
+  <si>
+    <t>CA de Nacido Vivo</t>
+  </si>
+  <si>
+    <t>Nacido vivo</t>
+  </si>
+  <si>
+    <t>CA de Defuncion</t>
+  </si>
+  <si>
+    <t>Defuncion</t>
+  </si>
+  <si>
+    <t>Sin uso</t>
+  </si>
+  <si>
+    <t>Asignado</t>
+  </si>
+  <si>
+    <t>Guardado</t>
+  </si>
+  <si>
+    <t>Extraviado</t>
+  </si>
+  <si>
+    <t>Anulado</t>
+  </si>
+  <si>
+    <t>Con incongruencias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +97,21 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -89,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -99,6 +146,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,16 +431,19 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -399,10 +451,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -420,6 +472,128 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Estados!$A$2:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Tipos!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>